<commit_message>
updated up potted plants
</commit_message>
<xml_diff>
--- a/input/Exp.Individs.xlsx
+++ b/input/Exp.Individs.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/springfreeze/input/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12620" yWindow="3880" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,20 +13,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="60">
   <si>
     <t>Species</t>
   </si>
@@ -139,13 +134,85 @@
   </si>
   <si>
     <t>ACEPEN05_WM</t>
+  </si>
+  <si>
+    <t>ALNINC01_HF</t>
+  </si>
+  <si>
+    <t>ALNINC07_SH</t>
+  </si>
+  <si>
+    <t>ALNINC06_HF</t>
+  </si>
+  <si>
+    <t>ALNINC05_SH</t>
+  </si>
+  <si>
+    <t>ALNINC09_HF</t>
+  </si>
+  <si>
+    <t>ALNINC08_HF</t>
+  </si>
+  <si>
+    <t>ALNINC02_HF</t>
+  </si>
+  <si>
+    <t>ALNINC05_HF</t>
+  </si>
+  <si>
+    <t>ACEPEN12_HF</t>
+  </si>
+  <si>
+    <t>BETPOP05_HF</t>
+  </si>
+  <si>
+    <t>BETPOP01_HF</t>
+  </si>
+  <si>
+    <t>BETPOP04_HF</t>
+  </si>
+  <si>
+    <t>BETPOP03_HF</t>
+  </si>
+  <si>
+    <t>VIBCAS01_SH</t>
+  </si>
+  <si>
+    <t>VIBCAS05_SH</t>
+  </si>
+  <si>
+    <t>VIBCAS10_GR</t>
+  </si>
+  <si>
+    <t>VIBCAS07_WM</t>
+  </si>
+  <si>
+    <t>VIBCAS03_GR</t>
+  </si>
+  <si>
+    <t>VIBCAS08_WM</t>
+  </si>
+  <si>
+    <t>VIBCAS09_SH</t>
+  </si>
+  <si>
+    <t>VIBCAS12_GR</t>
+  </si>
+  <si>
+    <t>CORCOR06_WM</t>
+  </si>
+  <si>
+    <t>CORCOR05_WM</t>
+  </si>
+  <si>
+    <t>UNK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,6 +222,22 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -177,14 +260,142 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="65">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -240,7 +451,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -275,7 +486,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -452,7 +663,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -469,9 +680,9 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +723,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -547,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -582,7 +793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -620,7 +831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -655,7 +866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -690,7 +901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -725,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -763,7 +974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -792,7 +1003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -821,7 +1032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -850,7 +1061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -879,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -905,7 +1116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -934,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -963,7 +1174,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -992,7 +1203,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1021,7 +1232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1047,7 +1258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1076,7 +1287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1105,7 +1316,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1116,7 +1327,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1130,7 +1341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1141,7 +1352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1155,7 +1366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1169,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1183,7 +1394,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1405,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1208,7 +1419,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1222,7 +1433,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1236,7 +1447,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1261,29 +1472,34 @@
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1306,7 +1522,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1326,7 +1542,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1346,7 +1562,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1366,7 +1582,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1386,7 +1602,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1406,7 +1622,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1426,7 +1642,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1446,7 +1662,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1466,7 +1682,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1486,7 +1702,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1506,7 +1722,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1526,7 +1742,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1546,7 +1762,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1566,7 +1782,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1586,7 +1802,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1606,7 +1822,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1626,7 +1842,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1646,7 +1862,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1666,7 +1882,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1686,7 +1902,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1706,7 +1922,7 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1723,11 +1939,1356 @@
         <v>42454</v>
       </c>
       <c r="F22" s="1">
-        <v>42661</v>
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E23" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F23" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E24" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F24" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E25" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F25" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E26" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F26" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E27" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F27" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E28" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F28" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E29" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F29" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E30" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F30" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E31" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F31" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E32" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F32" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E33" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F33" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E34" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F34" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E35" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F35" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E36" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F36" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E37" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F37" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E38" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F38" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E39" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F39" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E40" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F40" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E41" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F41" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E42" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F42" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="1">
+        <v>42068</v>
+      </c>
+      <c r="E43" s="1">
+        <v>42104</v>
+      </c>
+      <c r="F43" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="1">
+        <v>42012</v>
+      </c>
+      <c r="E44" s="1">
+        <v>42066</v>
+      </c>
+      <c r="F44" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="1">
+        <v>42012</v>
+      </c>
+      <c r="E45" s="1">
+        <v>42066</v>
+      </c>
+      <c r="F45" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="1">
+        <v>42012</v>
+      </c>
+      <c r="E46" s="1">
+        <v>42066</v>
+      </c>
+      <c r="F46" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="1">
+        <v>42012</v>
+      </c>
+      <c r="E47" s="1">
+        <v>42066</v>
+      </c>
+      <c r="F47" s="1">
+        <v>42663</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="1">
+        <v>42012</v>
+      </c>
+      <c r="E48" s="1">
+        <v>42066</v>
+      </c>
+      <c r="F48" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="1">
+        <v>42012</v>
+      </c>
+      <c r="E49" s="1">
+        <v>42066</v>
+      </c>
+      <c r="F49" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="1">
+        <v>42012</v>
+      </c>
+      <c r="E50" s="1">
+        <v>42066</v>
+      </c>
+      <c r="F50" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="1">
+        <v>42012</v>
+      </c>
+      <c r="E51" s="1">
+        <v>42066</v>
+      </c>
+      <c r="F51" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="1">
+        <v>42012</v>
+      </c>
+      <c r="E52" s="1">
+        <v>42066</v>
+      </c>
+      <c r="F52" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="1">
+        <v>41967</v>
+      </c>
+      <c r="E53" s="1">
+        <v>42065</v>
+      </c>
+      <c r="F53" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" s="1">
+        <v>41967</v>
+      </c>
+      <c r="E54" s="1">
+        <v>42065</v>
+      </c>
+      <c r="F54" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="1">
+        <v>41967</v>
+      </c>
+      <c r="E55" s="1">
+        <v>42065</v>
+      </c>
+      <c r="F55" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" s="1">
+        <v>41967</v>
+      </c>
+      <c r="E56" s="1">
+        <v>42065</v>
+      </c>
+      <c r="F56" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" s="1">
+        <v>41967</v>
+      </c>
+      <c r="E57" s="1">
+        <v>42065</v>
+      </c>
+      <c r="F57" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" s="1">
+        <v>41967</v>
+      </c>
+      <c r="E58" s="1">
+        <v>42065</v>
+      </c>
+      <c r="F58" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>49</v>
+      </c>
+      <c r="B59" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" s="1">
+        <v>41967</v>
+      </c>
+      <c r="E59" s="1">
+        <v>42065</v>
+      </c>
+      <c r="F59" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>49</v>
+      </c>
+      <c r="B60" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" s="1">
+        <v>41967</v>
+      </c>
+      <c r="E60" s="1">
+        <v>42065</v>
+      </c>
+      <c r="F60" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" s="1">
+        <v>41967</v>
+      </c>
+      <c r="E61" s="1">
+        <v>42065</v>
+      </c>
+      <c r="F61" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="1">
+        <v>42257</v>
+      </c>
+      <c r="D62" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E62" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F62" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>51</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="1">
+        <v>42257</v>
+      </c>
+      <c r="D63" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E63" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F63" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>52</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="1">
+        <v>42263</v>
+      </c>
+      <c r="D64" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E64" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F64" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>51</v>
+      </c>
+      <c r="B65" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="1">
+        <v>42257</v>
+      </c>
+      <c r="D65" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E65" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F65" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>52</v>
+      </c>
+      <c r="B66" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="1">
+        <v>42263</v>
+      </c>
+      <c r="D66" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E66" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F66" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="1">
+        <v>42256</v>
+      </c>
+      <c r="D67" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E67" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F67" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>52</v>
+      </c>
+      <c r="B68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" s="1">
+        <v>42263</v>
+      </c>
+      <c r="D68" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E68" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F68" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>52</v>
+      </c>
+      <c r="B69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="1">
+        <v>42263</v>
+      </c>
+      <c r="D69" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E69" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F69" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>51</v>
+      </c>
+      <c r="B70" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="1">
+        <v>42257</v>
+      </c>
+      <c r="D70" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E70" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F70" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>52</v>
+      </c>
+      <c r="B71" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="1">
+        <v>42263</v>
+      </c>
+      <c r="D71" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E71" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F71" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>51</v>
+      </c>
+      <c r="B72" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" s="1">
+        <v>42257</v>
+      </c>
+      <c r="D72" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E72" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F72" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>53</v>
+      </c>
+      <c r="B73" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="1">
+        <v>42256</v>
+      </c>
+      <c r="D73" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E73" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F73" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
+        <v>53</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="1">
+        <v>42256</v>
+      </c>
+      <c r="D74" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E74" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F74" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
+        <v>53</v>
+      </c>
+      <c r="B75" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" s="1">
+        <v>42256</v>
+      </c>
+      <c r="D75" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E75" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F75" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="1">
+        <v>42256</v>
+      </c>
+      <c r="D76" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E76" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F76" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>54</v>
+      </c>
+      <c r="B77" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" s="1">
+        <v>42263</v>
+      </c>
+      <c r="D77" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E77" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F77" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>54</v>
+      </c>
+      <c r="B78" t="s">
+        <v>12</v>
+      </c>
+      <c r="C78" s="1">
+        <v>42263</v>
+      </c>
+      <c r="D78" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E78" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F78" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" t="s">
+        <v>55</v>
+      </c>
+      <c r="B79" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" s="1">
+        <v>42255</v>
+      </c>
+      <c r="D79" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E79" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F79" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" t="s">
+        <v>54</v>
+      </c>
+      <c r="B80" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80" s="1">
+        <v>42263</v>
+      </c>
+      <c r="D80" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E80" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F80" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>56</v>
+      </c>
+      <c r="B81" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81" s="1">
+        <v>42257</v>
+      </c>
+      <c r="D81" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E81" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F81" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
+        <v>54</v>
+      </c>
+      <c r="B82" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" s="1">
+        <v>42263</v>
+      </c>
+      <c r="D82" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E82" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F82" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>56</v>
+      </c>
+      <c r="B83" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" s="1">
+        <v>42257</v>
+      </c>
+      <c r="D83" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E83" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F83" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>55</v>
+      </c>
+      <c r="B84" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" s="1">
+        <v>42255</v>
+      </c>
+      <c r="D84" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E84" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F84" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" t="s">
+        <v>49</v>
+      </c>
+      <c r="B85" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" s="1">
+        <v>42251</v>
+      </c>
+      <c r="D85" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E85" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F85" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>54</v>
+      </c>
+      <c r="B86" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" s="1">
+        <v>42263</v>
+      </c>
+      <c r="D86" s="1">
+        <v>42341</v>
+      </c>
+      <c r="E86" s="1">
+        <v>42418</v>
+      </c>
+      <c r="F86" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" t="s">
+        <v>57</v>
+      </c>
+      <c r="B87" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87" s="1">
+        <v>42226</v>
+      </c>
+      <c r="D87" s="1">
+        <v>42474</v>
+      </c>
+      <c r="E87" s="1">
+        <v>42488</v>
+      </c>
+      <c r="F87" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>58</v>
+      </c>
+      <c r="B88" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" s="1">
+        <v>42226</v>
+      </c>
+      <c r="D88" s="1">
+        <v>42474</v>
+      </c>
+      <c r="E88" s="1">
+        <v>42488</v>
+      </c>
+      <c r="F88" s="1">
+        <v>42667</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>57</v>
+      </c>
+      <c r="B89" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" s="1">
+        <v>42226</v>
+      </c>
+      <c r="D89" s="1">
+        <v>42474</v>
+      </c>
+      <c r="E89" s="1">
+        <v>42488</v>
+      </c>
+      <c r="F89" s="1">
+        <v>42667</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>